<commit_message>
Finishing the Location check
</commit_message>
<xml_diff>
--- a/src/main/resources/res1.xlsx
+++ b/src/main/resources/res1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="1" xr2:uid="{E198977B-E3B3-E340-BF34-C8569A0DE0CC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{E198977B-E3B3-E340-BF34-C8569A0DE0CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -548,8 +548,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -577,7 +577,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -594,7 +594,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -633,13 +633,13 @@
         <v>17</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>18</v>
@@ -667,7 +667,7 @@
         <v>22</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>1</v>
@@ -730,7 +730,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>28</v>
       </c>
@@ -803,10 +803,12 @@
     <filterColumn colId="4">
       <filters>
         <filter val="SHOT"/>
+        <filter val="SHOT 2"/>
       </filters>
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -814,8 +816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AD36675-E5C2-2B44-AF39-4DE63F77B108}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -871,7 +873,7 @@
         <v>37</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="D3">
         <v>3</v>
@@ -914,7 +916,7 @@
         <v>7</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E5">
         <v>0</v>

</xml_diff>